<commit_message>
Adjusted bd values to print month ending values
</commit_message>
<xml_diff>
--- a/src/assets/Book2.xlsx
+++ b/src/assets/Book2.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\manu0\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\BDConverter\src\assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{B7C53A20-5B80-4860-8AC7-412E317D4CAF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC3224A4-6198-471A-96E1-F787BDF37D3A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1620" yWindow="2592" windowWidth="17280" windowHeight="8964" xr2:uid="{23BB210A-5851-41AA-A11C-30EBE22EBCC0}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{23BB210A-5851-41AA-A11C-30EBE22EBCC0}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -23,9 +23,7 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
         <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
       </xcalcf:calcFeatures>
@@ -133,9 +131,6 @@
     <t>Nov21</t>
   </si>
   <si>
-    <t>Dec 21</t>
-  </si>
-  <si>
     <t>"1BD"</t>
   </si>
   <si>
@@ -320,6 +315,9 @@
   </si>
   <si>
     <t>1/27</t>
+  </si>
+  <si>
+    <t>Dec21</t>
   </si>
 </sst>
 </file>
@@ -681,12 +679,12 @@
   <dimension ref="A1:C37"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C37" sqref="C37"/>
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -694,10 +692,10 @@
         <v>31</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -705,10 +703,10 @@
         <v>2</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>17</v>
       </c>
@@ -716,10 +714,10 @@
         <v>3</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>18</v>
       </c>
@@ -727,10 +725,10 @@
         <v>4</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>20</v>
       </c>
@@ -738,10 +736,10 @@
         <v>5</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>19</v>
       </c>
@@ -749,10 +747,10 @@
         <v>6</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>21</v>
       </c>
@@ -760,10 +758,10 @@
         <v>7</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>22</v>
       </c>
@@ -771,10 +769,10 @@
         <v>8</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>23</v>
       </c>
@@ -782,10 +780,10 @@
         <v>9</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>24</v>
       </c>
@@ -793,10 +791,10 @@
         <v>10</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>25</v>
       </c>
@@ -804,10 +802,10 @@
         <v>11</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>26</v>
       </c>
@@ -815,10 +813,10 @@
         <v>12</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>27</v>
       </c>
@@ -826,10 +824,10 @@
         <v>13</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>28</v>
       </c>
@@ -837,10 +835,10 @@
         <v>14</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>29</v>
       </c>
@@ -848,10 +846,10 @@
         <v>15</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>30</v>
       </c>
@@ -859,238 +857,238 @@
         <v>16</v>
       </c>
       <c r="C16" s="1" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>32</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="C17" s="1" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A17" t="s">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
         <v>33</v>
       </c>
-      <c r="B17" s="1" t="s">
+      <c r="B18" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="C17" s="1" t="s">
+      <c r="C18" s="1" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A18" t="s">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
         <v>34</v>
       </c>
-      <c r="B18" s="1" t="s">
+      <c r="B19" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="C18" s="1" t="s">
+      <c r="C19" s="1" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A19" t="s">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
         <v>35</v>
       </c>
-      <c r="B19" s="1" t="s">
+      <c r="B20" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="C19" s="1" t="s">
+      <c r="C20" s="1" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A20" t="s">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
         <v>36</v>
       </c>
-      <c r="B20" s="1" t="s">
+      <c r="B21" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="C20" s="1" t="s">
+      <c r="C21" s="1" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A21" t="s">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
         <v>37</v>
       </c>
-      <c r="B21" s="1" t="s">
+      <c r="B22" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="C21" s="1" t="s">
+      <c r="C22" s="1" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>38</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="C23" s="1" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A22" t="s">
-        <v>38</v>
-      </c>
-      <c r="B22" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="C22" s="1" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A23" t="s">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
         <v>39</v>
       </c>
-      <c r="B23" s="1" t="s">
+      <c r="B24" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="C23" s="1" t="s">
+      <c r="C24" s="1" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A24" t="s">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
         <v>40</v>
       </c>
-      <c r="B24" s="1" t="s">
+      <c r="B25" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="C24" s="1" t="s">
+      <c r="C25" s="1" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A25" t="s">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
         <v>41</v>
       </c>
-      <c r="B25" s="1" t="s">
+      <c r="B26" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="C25" s="1" t="s">
+      <c r="C26" s="1" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A26" t="s">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
         <v>42</v>
       </c>
-      <c r="B26" s="1" t="s">
+      <c r="B27" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="C26" s="1" t="s">
+      <c r="C27" s="1" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A27" t="s">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
         <v>43</v>
       </c>
-      <c r="B27" s="1" t="s">
+      <c r="B28" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="C27" s="1" t="s">
+      <c r="C28" s="1" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A28" t="s">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
         <v>44</v>
       </c>
-      <c r="B28" s="1" t="s">
+      <c r="B29" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="C28" s="1" t="s">
+      <c r="C29" s="1" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A29" t="s">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
         <v>45</v>
       </c>
-      <c r="B29" s="1" t="s">
+      <c r="B30" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="C29" s="1" t="s">
+      <c r="C30" s="1" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A30" t="s">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
         <v>46</v>
       </c>
-      <c r="B30" s="1" t="s">
+      <c r="B31" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="C30" s="1" t="s">
+      <c r="C31" s="1" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A31" t="s">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
         <v>47</v>
       </c>
-      <c r="B31" s="1" t="s">
+      <c r="B32" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="C31" s="1" t="s">
+      <c r="C32" s="1" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A32" t="s">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
         <v>48</v>
       </c>
-      <c r="B32" s="1" t="s">
+      <c r="B33" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="C32" s="1" t="s">
+      <c r="C33" s="1" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A33" t="s">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
         <v>49</v>
       </c>
-      <c r="B33" s="1" t="s">
+      <c r="B34" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="C33" s="1" t="s">
+      <c r="C34" s="1" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A34" t="s">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
         <v>50</v>
       </c>
-      <c r="B34" s="1" t="s">
+      <c r="B35" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="C34" s="1" t="s">
+      <c r="C35" s="1" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A35" t="s">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
         <v>51</v>
       </c>
-      <c r="B35" s="1" t="s">
+      <c r="B36" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="C35" s="1" t="s">
+      <c r="C36" s="1" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A36" t="s">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
         <v>52</v>
       </c>
-      <c r="B36" s="1" t="s">
+      <c r="B37" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="C36" s="1" t="s">
+      <c r="C37" s="1" t="s">
         <v>93</v>
-      </c>
-    </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A37" t="s">
-        <v>53</v>
-      </c>
-      <c r="B37" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="C37" s="1" t="s">
-        <v>94</v>
       </c>
     </row>
   </sheetData>

</xml_diff>